<commit_message>
Corrección de etiquetas y formato de año
Corregí las etiquetas para estandarizar con el formato solicitado por el LEMA. Cambié el formato de año de YY a YYYY
</commit_message>
<xml_diff>
--- a/datos/Cajititlán_Env.xlsx
+++ b/datos/Cajititlán_Env.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccopi\Desktop\PP\Caji\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A3A94E-FCB5-4CFA-ABEB-1CA6DA007D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F0194C-1C90-4322-AB2F-5C969068D47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{23288B8C-CFF6-477E-BC6E-3C842449D796}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{23288B8C-CFF6-477E-BC6E-3C842449D796}"/>
   </bookViews>
   <sheets>
     <sheet name="Env" sheetId="1" r:id="rId1"/>
     <sheet name="EnvP" sheetId="4" r:id="rId2"/>
     <sheet name="Junk" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2110,52 +2110,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2185,13 +2155,43 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2514,7 +2514,7 @@
   </sheetPr>
   <dimension ref="A1:AZ338"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -2602,162 +2602,162 @@
       <c r="AZ1"/>
     </row>
     <row r="2" spans="1:52" s="118" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="158" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="160" t="s">
+      <c r="A2" s="148" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="162" t="s">
+      <c r="C2" s="152" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="164" t="s">
+      <c r="D2" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="166" t="s">
+      <c r="E2" s="156" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="152"/>
-      <c r="G2" s="152" t="s">
+      <c r="F2" s="142"/>
+      <c r="G2" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="152"/>
-      <c r="I2" s="152" t="s">
+      <c r="H2" s="142"/>
+      <c r="I2" s="142" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="152"/>
+      <c r="J2" s="142"/>
       <c r="K2" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="152" t="s">
+      <c r="L2" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="152" t="s">
+      <c r="M2" s="142" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="154" t="s">
+      <c r="N2" s="157" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="156" t="s">
+      <c r="O2" s="159" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="144" t="s">
+      <c r="P2" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="144" t="s">
+      <c r="Q2" s="146" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="144" t="s">
+      <c r="R2" s="146" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="144" t="s">
+      <c r="S2" s="146" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="144" t="s">
+      <c r="T2" s="146" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="150" t="s">
+      <c r="U2" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="V2" s="146" t="s">
+      <c r="V2" s="164" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="148" t="s">
+      <c r="W2" s="166" t="s">
         <v>17</v>
       </c>
-      <c r="X2" s="148" t="s">
+      <c r="X2" s="166" t="s">
         <v>19</v>
       </c>
-      <c r="Y2" s="148" t="s">
+      <c r="Y2" s="166" t="s">
         <v>20</v>
       </c>
-      <c r="Z2" s="148" t="s">
+      <c r="Z2" s="166" t="s">
         <v>21</v>
       </c>
-      <c r="AA2" s="148" t="s">
+      <c r="AA2" s="166" t="s">
         <v>22</v>
       </c>
-      <c r="AB2" s="142" t="s">
+      <c r="AB2" s="162" t="s">
         <v>23</v>
       </c>
-      <c r="AC2" s="142" t="s">
+      <c r="AC2" s="162" t="s">
         <v>24</v>
       </c>
-      <c r="AD2" s="142" t="s">
+      <c r="AD2" s="162" t="s">
         <v>25</v>
       </c>
-      <c r="AE2" s="144" t="s">
+      <c r="AE2" s="146" t="s">
         <v>54</v>
       </c>
-      <c r="AF2" s="144" t="s">
+      <c r="AF2" s="146" t="s">
         <v>55</v>
       </c>
-      <c r="AG2" s="144" t="s">
+      <c r="AG2" s="146" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="144" t="s">
+      <c r="AH2" s="146" t="s">
         <v>57</v>
       </c>
-      <c r="AI2" s="144" t="s">
+      <c r="AI2" s="146" t="s">
         <v>58</v>
       </c>
-      <c r="AJ2" s="144" t="s">
+      <c r="AJ2" s="146" t="s">
         <v>59</v>
       </c>
-      <c r="AK2" s="144" t="s">
+      <c r="AK2" s="146" t="s">
         <v>60</v>
       </c>
-      <c r="AL2" s="144" t="s">
+      <c r="AL2" s="146" t="s">
         <v>61</v>
       </c>
-      <c r="AM2" s="144" t="s">
+      <c r="AM2" s="146" t="s">
         <v>62</v>
       </c>
-      <c r="AN2" s="144" t="s">
+      <c r="AN2" s="146" t="s">
         <v>63</v>
       </c>
-      <c r="AO2" s="144" t="s">
+      <c r="AO2" s="146" t="s">
         <v>64</v>
       </c>
-      <c r="AP2" s="144" t="s">
+      <c r="AP2" s="146" t="s">
         <v>65</v>
       </c>
-      <c r="AQ2" s="152" t="s">
+      <c r="AQ2" s="142" t="s">
         <v>66</v>
       </c>
-      <c r="AR2" s="152" t="s">
+      <c r="AR2" s="142" t="s">
         <v>67</v>
       </c>
-      <c r="AS2" s="152" t="s">
+      <c r="AS2" s="142" t="s">
         <v>68</v>
       </c>
-      <c r="AT2" s="152" t="s">
+      <c r="AT2" s="142" t="s">
         <v>69</v>
       </c>
-      <c r="AU2" s="152" t="s">
+      <c r="AU2" s="142" t="s">
         <v>70</v>
       </c>
-      <c r="AV2" s="152" t="s">
+      <c r="AV2" s="142" t="s">
         <v>71</v>
       </c>
-      <c r="AW2" s="152" t="s">
+      <c r="AW2" s="142" t="s">
         <v>72</v>
       </c>
-      <c r="AX2" s="152" t="s">
+      <c r="AX2" s="142" t="s">
         <v>73</v>
       </c>
-      <c r="AY2" s="152" t="s">
+      <c r="AY2" s="142" t="s">
         <v>74</v>
       </c>
-      <c r="AZ2" s="168" t="s">
+      <c r="AZ2" s="144" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:52" s="118" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="159"/>
-      <c r="B3" s="161"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="165"/>
+      <c r="A3" s="149"/>
+      <c r="B3" s="151"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="155"/>
       <c r="E3" s="112" t="s">
         <v>26</v>
       </c>
@@ -2779,47 +2779,47 @@
       <c r="K3" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="153"/>
-      <c r="M3" s="153"/>
-      <c r="N3" s="155"/>
-      <c r="O3" s="157"/>
-      <c r="P3" s="145"/>
-      <c r="Q3" s="145"/>
-      <c r="R3" s="145"/>
-      <c r="S3" s="145"/>
-      <c r="T3" s="145"/>
-      <c r="U3" s="151"/>
-      <c r="V3" s="147"/>
-      <c r="W3" s="149"/>
-      <c r="X3" s="149"/>
-      <c r="Y3" s="149"/>
-      <c r="Z3" s="149"/>
-      <c r="AA3" s="149"/>
-      <c r="AB3" s="143"/>
-      <c r="AC3" s="143"/>
-      <c r="AD3" s="143"/>
-      <c r="AE3" s="167"/>
-      <c r="AF3" s="167"/>
-      <c r="AG3" s="167"/>
-      <c r="AH3" s="167"/>
-      <c r="AI3" s="167"/>
-      <c r="AJ3" s="167"/>
-      <c r="AK3" s="167"/>
-      <c r="AL3" s="167"/>
-      <c r="AM3" s="167"/>
-      <c r="AN3" s="167"/>
-      <c r="AO3" s="167"/>
-      <c r="AP3" s="167"/>
-      <c r="AQ3" s="153"/>
-      <c r="AR3" s="153"/>
-      <c r="AS3" s="153"/>
-      <c r="AT3" s="153"/>
-      <c r="AU3" s="153"/>
-      <c r="AV3" s="153"/>
-      <c r="AW3" s="153"/>
-      <c r="AX3" s="153"/>
-      <c r="AY3" s="153"/>
-      <c r="AZ3" s="169"/>
+      <c r="L3" s="143"/>
+      <c r="M3" s="143"/>
+      <c r="N3" s="158"/>
+      <c r="O3" s="160"/>
+      <c r="P3" s="161"/>
+      <c r="Q3" s="161"/>
+      <c r="R3" s="161"/>
+      <c r="S3" s="161"/>
+      <c r="T3" s="161"/>
+      <c r="U3" s="169"/>
+      <c r="V3" s="165"/>
+      <c r="W3" s="167"/>
+      <c r="X3" s="167"/>
+      <c r="Y3" s="167"/>
+      <c r="Z3" s="167"/>
+      <c r="AA3" s="167"/>
+      <c r="AB3" s="163"/>
+      <c r="AC3" s="163"/>
+      <c r="AD3" s="163"/>
+      <c r="AE3" s="147"/>
+      <c r="AF3" s="147"/>
+      <c r="AG3" s="147"/>
+      <c r="AH3" s="147"/>
+      <c r="AI3" s="147"/>
+      <c r="AJ3" s="147"/>
+      <c r="AK3" s="147"/>
+      <c r="AL3" s="147"/>
+      <c r="AM3" s="147"/>
+      <c r="AN3" s="147"/>
+      <c r="AO3" s="147"/>
+      <c r="AP3" s="147"/>
+      <c r="AQ3" s="143"/>
+      <c r="AR3" s="143"/>
+      <c r="AS3" s="143"/>
+      <c r="AT3" s="143"/>
+      <c r="AU3" s="143"/>
+      <c r="AV3" s="143"/>
+      <c r="AW3" s="143"/>
+      <c r="AX3" s="143"/>
+      <c r="AY3" s="143"/>
+      <c r="AZ3" s="145"/>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.3">
       <c r="A4" s="44">
@@ -46969,40 +46969,6 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="AT2:AT3"/>
-    <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="AQ2:AQ3"/>
-    <mergeCell ref="AR2:AR3"/>
-    <mergeCell ref="AS2:AS3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
     <mergeCell ref="AB2:AB3"/>
     <mergeCell ref="AC2:AC3"/>
     <mergeCell ref="AD2:AD3"/>
@@ -47017,6 +46983,40 @@
     <mergeCell ref="Z2:Z3"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="U2:U3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AR2:AR3"/>
+    <mergeCell ref="AS2:AS3"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="AT2:AT3"/>
+    <mergeCell ref="AU2:AU3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AX2:AX3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -47028,8 +47028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F147FEA-BF3F-4631-8EB6-2C924D13CB49}">
   <dimension ref="A1:AQ287"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>